<commit_message>
Start of model-specific behavior
</commit_message>
<xml_diff>
--- a/data/notes/models.xlsx
+++ b/data/notes/models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1695</v>
+        <v>1965</v>
       </c>
       <c r="C2">
         <v>1968</v>

</xml_diff>

<commit_message>
Properly limit BSW to models supported
</commit_message>
<xml_diff>
--- a/data/notes/models.xlsx
+++ b/data/notes/models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="0" windowWidth="51200" windowHeight="27240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Model</t>
   </si>
@@ -564,7 +564,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -762,7 +762,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -803,6 +803,9 @@
       <c r="A5" t="s">
         <v>35</v>
       </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">

</xml_diff>